<commit_message>
LMDI: Merge pull request #34 from folkehelseinstituttet/issue/32
Ny versjon 1.0.7 bda9267a9073f17b6616cb2e434dfa97e8667cb1
</commit_message>
<xml_diff>
--- a/currentbuild/CodeSystem-LokalLegemiddelkatalogCodeSystem.xlsx
+++ b/currentbuild/CodeSystem-LokalLegemiddelkatalogCodeSystem.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.0.4</t>
+    <t>1.0.7</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-09-18T12:15:28+00:00</t>
+    <t>2025-09-30T09:52:39+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>